<commit_message>
Addressed Issue #5. Provided a provision to input optional email and hash details. Updated message with date.
</commit_message>
<xml_diff>
--- a/exe/SampleInput.xlsx
+++ b/exe/SampleInput.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h224423\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A_Data\Projects\eclipse-workspace\MessageSender\exe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -32,6 +32,9 @@
     <t>Balance</t>
   </si>
   <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
     <t>name1</t>
   </si>
   <si>
@@ -39,15 +42,6 @@
   </si>
   <si>
     <t>100</t>
-  </si>
-  <si>
-    <t>name2</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
   </si>
 </sst>
 </file>
@@ -400,9 +394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -413,7 +409,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -424,24 +420,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>